<commit_message>
Correct functionality in admin app
</commit_message>
<xml_diff>
--- a/OnlineLibraryAdmin/OnlineLibraryAdmin/files/Authors.xlsx
+++ b/OnlineLibraryAdmin/OnlineLibraryAdmin/files/Authors.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elena\Faks\Shesti semestar\Integrirani sistemi\Proekt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4658C7A-8A49-40B3-9C2E-48CB1CDCE4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B9F602-BE4D-44B0-8FE8-BD6930A51E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,34 +27,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Riste</t>
-  </si>
-  <si>
-    <t>Ristov</t>
-  </si>
-  <si>
-    <t>Vale</t>
-  </si>
-  <si>
-    <t>Valeva</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>Anceva</t>
-  </si>
-  <si>
-    <t>Hristijan</t>
-  </si>
-  <si>
-    <t>Hristov</t>
-  </si>
-  <si>
-    <t>Todor</t>
-  </si>
-  <si>
-    <t>Trajkov</t>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Benet</t>
+  </si>
+  <si>
+    <t>Ethan</t>
+  </si>
+  <si>
+    <t>Harris</t>
+  </si>
+  <si>
+    <t>Lily</t>
+  </si>
+  <si>
+    <t>Thomson</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Walker</t>
+  </si>
+  <si>
+    <t>Liam</t>
+  </si>
+  <si>
+    <t>Edwards</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>